<commit_message>
add example for API test
</commit_message>
<xml_diff>
--- a/csharp/QA.AutomatedTests/QA.Common/Artifacts/ConfigurationStore.xlsx
+++ b/csharp/QA.AutomatedTests/QA.Common/Artifacts/ConfigurationStore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JamesLe\Projects\dohuul\demo\csharp\QA.AutomatedTests\QA.Common\Artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CA9A72-90BB-43CB-8181-E869C0CDBFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E53A911-9AD2-4F38-B19C-D8D9DABDA5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="3735" windowWidth="23205" windowHeight="11295" activeTab="1" xr2:uid="{64050745-601B-4068-901B-CC4E98E03070}"/>
+    <workbookView xWindow="7380" yWindow="3735" windowWidth="23205" windowHeight="11295" xr2:uid="{64050745-601B-4068-901B-CC4E98E03070}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductUrls" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>https://66704af90900b5f8724a1c06.mockapi.io/api/v1/user</t>
   </si>
   <si>
-    <t>JamesMockService</t>
-  </si>
-  <si>
     <t>Environment</t>
   </si>
   <si>
@@ -68,6 +65,9 @@
   </si>
   <si>
     <t>NAME=jim test&amp;AGE=33</t>
+  </si>
+  <si>
+    <t>JamesTestService</t>
   </si>
 </sst>
 </file>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{226617B1-9FB0-4F21-A346-0423F4BB140C}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,10 +434,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -448,7 +448,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -485,7 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018082C5-40BB-41F2-85C4-BDBFBDB39E80}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -498,13 +498,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -512,10 +512,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,10 +523,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -534,10 +534,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>